<commit_message>
Stinger and Febreze tax validation code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Stinger/Taxaddresscode.xlsx
+++ b/src/test/resources/TestData/Stinger/Taxaddresscode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workjee\New folder\1\HoT-digital\HoT-digital\src\test\resources\TestData\Stinger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkJEE!\stinger tax code 22-09-2021\tax\HoT-digital\src\test\resources\TestData\Stinger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4C6BD3-2167-4412-A87E-BF2321761515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B6ED98-3164-4FBD-B29B-65768955BC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="11070" xr2:uid="{8A6B3A0F-54D1-4F06-8D67-2951571DD11A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A6B3A0F-54D1-4F06-8D67-2951571DD11A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1328,7 +1328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53772E61-919E-4A2B-8048-ECEF9203B94F}">
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -1336,7 +1336,7 @@
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>

</xml_diff>